<commit_message>
Tested keyboard and menu.
</commit_message>
<xml_diff>
--- a/Pangeo/Assets/Tests/VisualTests/VisualTests.xlsx
+++ b/Pangeo/Assets/Tests/VisualTests/VisualTests.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,20 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7180120\Documents\VRtualize-Pangeo\Pangeo\Assets\Tests\VisualTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8D90A6D6-B826-4540-8E96-DA0E3079974B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CB59A9-EE52-4DA2-AD23-467B9C3D78B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Keyboard Movement" sheetId="1" r:id="rId1"/>
     <sheet name="VR Movement" sheetId="7" r:id="rId2"/>
+    <sheet name="Main Menu Test" sheetId="9" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="80000"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="75">
   <si>
     <t>Test Case Description</t>
   </si>
@@ -200,12 +203,66 @@
   </si>
   <si>
     <t>Touch south quadrant of the right controller trackpad</t>
+  </si>
+  <si>
+    <t>Touch northeast quadrant of the left controller trackpad</t>
+  </si>
+  <si>
+    <t>Touch northwest quadrant of the left controller trackpad</t>
+  </si>
+  <si>
+    <t>Camera moves up and to the left</t>
+  </si>
+  <si>
+    <t>Camera moves up and to the right</t>
+  </si>
+  <si>
+    <t>Touch southwest quadrant of the left controller trackpad</t>
+  </si>
+  <si>
+    <t>Camera moves down and to the left</t>
+  </si>
+  <si>
+    <t>Touch southeast quadrant of the left controller trackpad</t>
+  </si>
+  <si>
+    <t>Camera moves down and to the right</t>
+  </si>
+  <si>
+    <t>Test Main Menu functionality</t>
+  </si>
+  <si>
+    <t>VT_003</t>
+  </si>
+  <si>
+    <t>Verify that main menu controls acts as expected</t>
+  </si>
+  <si>
+    <t>Run "MainMenu" scene in Play Mode</t>
+  </si>
+  <si>
+    <t>Select the Coordinates button</t>
+  </si>
+  <si>
+    <t>Coordinates panel opens</t>
+  </si>
+  <si>
+    <t>Menu resets back to main menu</t>
+  </si>
+  <si>
+    <t>Select the Back button</t>
+  </si>
+  <si>
+    <t>Select the Controls button</t>
+  </si>
+  <si>
+    <t>Controls panel opens</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmmm\ d\,\ yyyy"/>
   </numFmts>
@@ -345,7 +402,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -393,6 +450,21 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -402,86 +474,197 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="17">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -756,11 +939,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -771,48 +954,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="30"/>
+      <c r="B1" s="32"/>
       <c r="C1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="30"/>
-      <c r="F1" s="18" t="s">
+      <c r="E1" s="32"/>
+      <c r="F1" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="30"/>
+      <c r="B2" s="32"/>
       <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="26" t="s">
+      <c r="E2" s="32"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="30"/>
-      <c r="J2" s="37" t="s">
+      <c r="I2" s="32"/>
+      <c r="J2" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="38"/>
+      <c r="K2" s="35"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
@@ -828,10 +1011,10 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="38"/>
       <c r="C4" s="13"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -856,29 +1039,25 @@
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="26" t="s">
+      <c r="B6" s="38"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="27"/>
-      <c r="F6" s="40">
-        <v>43905</v>
-      </c>
-      <c r="G6" s="41"/>
-      <c r="H6" s="26" t="s">
+      <c r="E6" s="38"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="27"/>
-      <c r="J6" s="22" t="s">
+      <c r="I6" s="38"/>
+      <c r="J6" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="K6" s="22"/>
+      <c r="K6" s="25"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
@@ -897,94 +1076,94 @@
       <c r="A8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
       <c r="E8" s="9"/>
       <c r="F8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>1</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="24"/>
       <c r="E9" s="3"/>
       <c r="F9" s="11">
         <v>1</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="19"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="24"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>2</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="24"/>
       <c r="E10" s="3"/>
       <c r="F10" s="11">
         <v>2</v>
       </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="19"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="24"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>3</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="24"/>
       <c r="E11" s="3"/>
       <c r="F11" s="11">
         <v>3</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="19"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="24"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>4</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="24"/>
       <c r="E12" s="3"/>
       <c r="F12" s="11">
         <v>4</v>
       </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="19"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="24"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
@@ -1017,245 +1196,248 @@
       <c r="K14" s="4"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="28" t="s">
+      <c r="C16" s="42"/>
+      <c r="D16" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="20" t="s">
+      <c r="E16" s="45"/>
+      <c r="F16" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="20" t="s">
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="35"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
     </row>
     <row r="18" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>1</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="25" t="s">
+      <c r="C18" s="36"/>
+      <c r="D18" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="25"/>
-      <c r="F18" s="17" t="s">
+      <c r="E18" s="29"/>
+      <c r="F18" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="17" t="s">
+      <c r="G18" s="23"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="J18" s="18"/>
-      <c r="K18" s="19"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="24"/>
     </row>
     <row r="19" spans="1:11" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>2</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="42" t="s">
+      <c r="C19" s="21"/>
+      <c r="D19" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="43"/>
-      <c r="F19" s="17" t="s">
+      <c r="E19" s="21"/>
+      <c r="F19" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="17" t="s">
+      <c r="G19" s="23"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="J19" s="18"/>
-      <c r="K19" s="19"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="24"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>6</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="39"/>
-      <c r="D20" s="25" t="s">
+      <c r="C20" s="30"/>
+      <c r="D20" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="25"/>
-      <c r="F20" s="17" t="s">
+      <c r="E20" s="29"/>
+      <c r="F20" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="17" t="s">
+      <c r="G20" s="23"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="J20" s="18"/>
-      <c r="K20" s="19"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="24"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>7</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="39"/>
-      <c r="D21" s="25" t="s">
+      <c r="C21" s="30"/>
+      <c r="D21" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="25"/>
-      <c r="F21" s="17" t="s">
+      <c r="E21" s="29"/>
+      <c r="F21" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="18"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="17" t="s">
+      <c r="G21" s="23"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="J21" s="18"/>
-      <c r="K21" s="19"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="24"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
         <v>8</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="39"/>
-      <c r="D22" s="25" t="s">
+      <c r="C22" s="30"/>
+      <c r="D22" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="25"/>
-      <c r="F22" s="17" t="s">
+      <c r="E22" s="29"/>
+      <c r="F22" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G22" s="18"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="17" t="s">
+      <c r="G22" s="23"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="J22" s="18"/>
-      <c r="K22" s="19"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="24"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
         <v>9</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="39"/>
-      <c r="D23" s="25" t="s">
+      <c r="C23" s="30"/>
+      <c r="D23" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="25"/>
-      <c r="F23" s="17" t="s">
+      <c r="E23" s="29"/>
+      <c r="F23" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G23" s="18"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="17" t="s">
+      <c r="G23" s="23"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="J23" s="18"/>
-      <c r="K23" s="19"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="24"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <v>10</v>
       </c>
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="43"/>
-      <c r="D24" s="42" t="s">
+      <c r="C24" s="21"/>
+      <c r="D24" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="E24" s="43"/>
-      <c r="F24" s="17" t="s">
+      <c r="E24" s="21"/>
+      <c r="F24" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G24" s="18"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="17" t="s">
+      <c r="G24" s="23"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="J24" s="18"/>
-      <c r="K24" s="19"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="24"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
         <v>11</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="45"/>
-      <c r="D25" s="22" t="s">
+      <c r="C25" s="26"/>
+      <c r="D25" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="E25" s="22"/>
-      <c r="F25" s="17" t="s">
+      <c r="E25" s="25"/>
+      <c r="F25" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G25" s="18"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="17" t="s">
+      <c r="G25" s="23"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="J25" s="18"/>
-      <c r="K25" s="19"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="61">
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="F16:H17"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="D16:E17"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="I16:K17"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="G10:K10"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D2:E2"/>
@@ -1272,35 +1454,46 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D25:E25"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="B16:C17"/>
     <mergeCell ref="D18:E18"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="D16:E17"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F20:H20"/>
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="F22:H22"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="I16:K17"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="G10:K10"/>
     <mergeCell ref="F23:H23"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="F16:H17"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:K19"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="I18:K99">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Not executed">
+      <formula>NOT(ISERROR(SEARCH("Not executed",I18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",I18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",I18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Suspended">
+      <formula>NOT(ISERROR(SEARCH("Suspended",I18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -1308,11 +1501,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25:H25"/>
+    <sheetView topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20:K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1323,48 +1516,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="30"/>
+      <c r="B1" s="32"/>
       <c r="C1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="30"/>
-      <c r="F1" s="18" t="s">
+      <c r="E1" s="32"/>
+      <c r="F1" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="30"/>
+      <c r="B2" s="32"/>
       <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="26" t="s">
+      <c r="E2" s="32"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="30"/>
-      <c r="J2" s="37" t="s">
+      <c r="I2" s="32"/>
+      <c r="J2" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="38"/>
+      <c r="K2" s="35"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
@@ -1380,10 +1573,10 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="38"/>
       <c r="C4" s="13"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -1408,29 +1601,25 @@
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="26" t="s">
+      <c r="B6" s="38"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="27"/>
-      <c r="F6" s="40">
-        <v>43905</v>
-      </c>
-      <c r="G6" s="41"/>
-      <c r="H6" s="26" t="s">
+      <c r="E6" s="38"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="27"/>
-      <c r="J6" s="22" t="s">
+      <c r="I6" s="38"/>
+      <c r="J6" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="K6" s="22"/>
+      <c r="K6" s="25"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
@@ -1449,94 +1638,94 @@
       <c r="A8" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
       <c r="E8" s="9"/>
       <c r="F8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>1</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="24"/>
       <c r="E9" s="3"/>
       <c r="F9" s="11">
         <v>1</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="19"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="24"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>2</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="24"/>
       <c r="E10" s="3"/>
       <c r="F10" s="11">
         <v>2</v>
       </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="19"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="24"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>3</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="24"/>
       <c r="E11" s="3"/>
       <c r="F11" s="11">
         <v>3</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="19"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="24"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>4</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="24"/>
       <c r="E12" s="3"/>
       <c r="F12" s="11">
         <v>4</v>
       </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="19"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="24"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
@@ -1569,287 +1758,388 @@
       <c r="K14" s="4"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="28" t="s">
+      <c r="C16" s="42"/>
+      <c r="D16" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="20" t="s">
+      <c r="E16" s="45"/>
+      <c r="F16" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="20" t="s">
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="35"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
     </row>
     <row r="18" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>1</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="25" t="s">
+      <c r="C18" s="36"/>
+      <c r="D18" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="25"/>
-      <c r="F18" s="17" t="s">
+      <c r="E18" s="29"/>
+      <c r="F18" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="17" t="s">
+      <c r="G18" s="23"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="J18" s="18"/>
-      <c r="K18" s="19"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="24"/>
     </row>
     <row r="19" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>2</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="42" t="s">
+      <c r="C19" s="21"/>
+      <c r="D19" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E19" s="43"/>
-      <c r="F19" s="17" t="s">
+      <c r="E19" s="21"/>
+      <c r="F19" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="17" t="s">
+      <c r="G19" s="23"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="J19" s="18"/>
-      <c r="K19" s="19"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="24"/>
     </row>
     <row r="20" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>3</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="39"/>
-      <c r="D20" s="25" t="s">
+      <c r="C20" s="30"/>
+      <c r="D20" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="25"/>
-      <c r="F20" s="17" t="s">
+      <c r="E20" s="29"/>
+      <c r="F20" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="17" t="s">
+      <c r="G20" s="23"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="J20" s="18"/>
-      <c r="K20" s="19"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="24"/>
     </row>
     <row r="21" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>4</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="39"/>
-      <c r="D21" s="25" t="s">
+      <c r="C21" s="30"/>
+      <c r="D21" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="25"/>
-      <c r="F21" s="17" t="s">
+      <c r="E21" s="29"/>
+      <c r="F21" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="18"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="17" t="s">
+      <c r="G21" s="23"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="J21" s="18"/>
-      <c r="K21" s="19"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="24"/>
     </row>
     <row r="22" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
         <v>5</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="39"/>
-      <c r="D22" s="25" t="s">
+      <c r="C22" s="30"/>
+      <c r="D22" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="25"/>
-      <c r="F22" s="17" t="s">
+      <c r="E22" s="29"/>
+      <c r="F22" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G22" s="18"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="17" t="s">
+      <c r="G22" s="23"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="J22" s="18"/>
-      <c r="K22" s="19"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="24"/>
     </row>
     <row r="23" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
         <v>6</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="39"/>
-      <c r="D23" s="25" t="s">
+      <c r="C23" s="30"/>
+      <c r="D23" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="25"/>
-      <c r="F23" s="17" t="s">
+      <c r="E23" s="29"/>
+      <c r="F23" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G23" s="18"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="17" t="s">
+      <c r="G23" s="23"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="J23" s="18"/>
-      <c r="K23" s="19"/>
-    </row>
-    <row r="24" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J23" s="23"/>
+      <c r="K23" s="24"/>
+    </row>
+    <row r="24" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <v>7</v>
       </c>
-      <c r="B24" s="42"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="44"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="44"/>
-      <c r="K24" s="43"/>
-    </row>
-    <row r="25" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="30"/>
+      <c r="D24" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="29"/>
+      <c r="F24" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" s="23"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="J24" s="23"/>
+      <c r="K24" s="24"/>
+    </row>
+    <row r="25" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
         <v>8</v>
       </c>
-      <c r="B25" s="42"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="44"/>
-      <c r="K25" s="43"/>
-    </row>
-    <row r="26" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="30"/>
+      <c r="D25" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="29"/>
+      <c r="F25" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="23"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="J25" s="23"/>
+      <c r="K25" s="24"/>
+    </row>
+    <row r="26" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
         <v>9</v>
       </c>
-      <c r="B26" s="42"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="44"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="44"/>
-      <c r="K26" s="43"/>
-    </row>
-    <row r="27" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="30"/>
+      <c r="D26" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="29"/>
+      <c r="F26" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="23"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="J26" s="23"/>
+      <c r="K26" s="24"/>
+    </row>
+    <row r="27" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11">
         <v>10</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="43"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="44"/>
-      <c r="K27" s="43"/>
+      <c r="B27" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="30"/>
+      <c r="D27" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="29"/>
+      <c r="F27" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="23"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="J27" s="23"/>
+      <c r="K27" s="24"/>
     </row>
     <row r="28" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11">
         <v>11</v>
       </c>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="39"/>
-      <c r="D28" s="42" t="s">
+      <c r="C28" s="30"/>
+      <c r="D28" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="E28" s="43"/>
-      <c r="F28" s="17" t="s">
+      <c r="E28" s="21"/>
+      <c r="F28" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G28" s="18"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="17" t="s">
+      <c r="G28" s="23"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="J28" s="18"/>
-      <c r="K28" s="19"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="24"/>
     </row>
     <row r="29" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11">
         <v>12</v>
       </c>
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="39"/>
-      <c r="D29" s="22" t="s">
+      <c r="C29" s="30"/>
+      <c r="D29" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="22"/>
-      <c r="F29" s="17" t="s">
+      <c r="E29" s="25"/>
+      <c r="F29" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G29" s="18"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="17" t="s">
+      <c r="G29" s="23"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="J29" s="18"/>
-      <c r="K29" s="19"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="77">
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="D16:E17"/>
+    <mergeCell ref="F16:H17"/>
+    <mergeCell ref="I16:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:H29"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="I25:K25"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="F26:H26"/>
@@ -1858,6 +2148,476 @@
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="F27:H27"/>
     <mergeCell ref="I27:K27"/>
+  </mergeCells>
+  <conditionalFormatting sqref="I18:K99">
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",I18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="3" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",I18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="2" operator="containsText" text="Not executed">
+      <formula>NOT(ISERROR(SEARCH("Not executed",I18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="Suspended">
+      <formula>NOT(ISERROR(SEARCH("Suspended",I18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC9EC6C7-EC67-46E6-8BDB-9E6E149F83FC}">
+  <dimension ref="A1:K25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18:K18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="7" width="9.140625" style="2"/>
+    <col min="8" max="9" width="11.28515625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="32"/>
+      <c r="F1" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="24"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="32"/>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="32"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="32"/>
+      <c r="J2" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="35"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="38"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="38"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="38"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="38"/>
+      <c r="J6" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="25"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="11">
+        <v>1</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="23"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="11">
+        <v>1</v>
+      </c>
+      <c r="G9" s="22"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="24"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="11">
+        <v>2</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="23"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="11">
+        <v>2</v>
+      </c>
+      <c r="G10" s="22"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="24"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="11">
+        <v>3</v>
+      </c>
+      <c r="B11" s="22"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="11">
+        <v>3</v>
+      </c>
+      <c r="G11" s="22"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="24"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="11">
+        <v>4</v>
+      </c>
+      <c r="B12" s="22"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="11">
+        <v>4</v>
+      </c>
+      <c r="G12" s="22"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="24"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="42"/>
+      <c r="D16" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="45"/>
+      <c r="F16" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" s="47"/>
+      <c r="K16" s="47"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="42"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
+    </row>
+    <row r="18" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="11">
+        <v>1</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="36"/>
+      <c r="D18" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="29"/>
+      <c r="F18" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="23"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="J18" s="23"/>
+      <c r="K18" s="24"/>
+    </row>
+    <row r="19" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="11">
+        <v>2</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="21"/>
+      <c r="D19" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="21"/>
+      <c r="F19" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="23"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="J19" s="23"/>
+      <c r="K19" s="24"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="11">
+        <v>3</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="30"/>
+      <c r="D20" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="29"/>
+      <c r="F20" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="23"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="J20" s="23"/>
+      <c r="K20" s="24"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="11">
+        <v>4</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="30"/>
+      <c r="D21" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" s="29"/>
+      <c r="F21" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="23"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="J21" s="23"/>
+      <c r="K21" s="24"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="11">
+        <v>5</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="30"/>
+      <c r="D22" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="29"/>
+      <c r="F22" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="23"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="J22" s="23"/>
+      <c r="K22" s="24"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="11"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="24"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="11"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="24"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="11"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="61">
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="F24:H24"/>
@@ -1866,14 +2626,6 @@
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="F25:H25"/>
     <mergeCell ref="I25:K25"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:H29"/>
-    <mergeCell ref="I29:K29"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="F22:H22"/>
@@ -1928,6 +2680,20 @@
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
   </mergeCells>
+  <conditionalFormatting sqref="I18:K99">
+    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="Pass">
+      <formula>NOT(ISERROR(SEARCH("Pass",I18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Fail">
+      <formula>NOT(ISERROR(SEARCH("Fail",I18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="Not executed">
+      <formula>NOT(ISERROR(SEARCH("Not executed",I18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Suspended">
+      <formula>NOT(ISERROR(SEARCH("Suspended",I18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>